<commit_message>
this is my new commite with readexcel class
</commit_message>
<xml_diff>
--- a/src/test/java/one/globalenglish/testData/LoginData.xlsx
+++ b/src/test/java/one/globalenglish/testData/LoginData.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VictorArunJoseph\Products\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC412DF-7A6D-457F-905B-378DA7176634}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{288CB808-79B4-4329-B094-98470ACFB5AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CB8AE96E-74F7-401B-BA20-15EB3278E860}"/>
+    <workbookView xWindow="5480" yWindow="3520" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{CB8AE96E-74F7-401B-BA20-15EB3278E860}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -46,16 +43,33 @@
   </si>
   <si>
     <t>Airtel@123</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Insightadmin</t>
+  </si>
+  <si>
+    <t>Insight_0217</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,15 +98,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CA692D-D5CB-4360-9241-59B088880DC8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -460,4 +477,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA60A0F-1B45-4442-8D2A-5472AB7DBD65}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AB453C0A-15E5-4A31-B94A-107CEF71A97D}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{3FC97519-3968-4577-8CE1-A7A4A9F67C57}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
moving my local code to gitlab
</commit_message>
<xml_diff>
--- a/src/test/java/one/globalenglish/testData/LoginData.xlsx
+++ b/src/test/java/one/globalenglish/testData/LoginData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{288CB808-79B4-4329-B094-98470ACFB5AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{64600B34-E7F7-476A-845E-6598BDF85BA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="3520" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{CB8AE96E-74F7-401B-BA20-15EB3278E860}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14440" windowHeight="9350" activeTab="1" xr2:uid="{CB8AE96E-74F7-401B-BA20-15EB3278E860}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>